<commit_message>
Various updates toward carbon
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/I2C_Timing.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/I2C_Timing.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet4!$A$31:$H$57</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="162">
   <si>
     <t>Initialization</t>
   </si>
@@ -248,12 +251,6 @@
     <t>else</t>
   </si>
   <si>
-    <t>if all_config_bits_set goto Acquisition</t>
-  </si>
-  <si>
-    <t>goto Read Configuration</t>
-  </si>
-  <si>
     <t>Delay 85000 us</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
     <t>SelectAll(0)</t>
   </si>
   <si>
-    <t>WriteRead(40,F3,3)</t>
-  </si>
-  <si>
     <t>WriteRead(77,0,3)</t>
   </si>
   <si>
@@ -317,21 +311,9 @@
     <t>If ESID(PTRHn) /= CurESID</t>
   </si>
   <si>
-    <t>If ESwitchMask(PTRHn) /= 0</t>
-  </si>
-  <si>
     <t>ESwitchMask &lt;= ( others =&gt; '0' );</t>
   </si>
   <si>
-    <t>ESwitchMask(ESwitchBit) &lt;= '1';</t>
-  </si>
-  <si>
-    <t>ISwitchMask &lt;= (others =&gt; '0');</t>
-  </si>
-  <si>
-    <t>ISwitchMask(ISWITCH_BIT(CurESID-1)) &lt;= '1';</t>
-  </si>
-  <si>
     <t>CurESID &lt;= ESID(PTRHn)</t>
   </si>
   <si>
@@ -375,6 +357,189 @@
   </si>
   <si>
     <t>ESB_array</t>
+  </si>
+  <si>
+    <t>If ESwitchAddr(CurESID) /= "0000000"</t>
+  </si>
+  <si>
+    <t>ESwitchMask(ESwitchBit(PTRHn)) &lt;= '1';</t>
+  </si>
+  <si>
+    <t>ISwitch &lt;= (others =&gt; '0');</t>
+  </si>
+  <si>
+    <t>ISwitch(ISwitchBit(CurESID)) &lt;= '1';</t>
+  </si>
+  <si>
+    <t>[ESID]</t>
+  </si>
+  <si>
+    <t>Or defined redundantly and checked with assertions during test.</t>
+  </si>
+  <si>
+    <t>clear all RAM</t>
+  </si>
+  <si>
+    <t>Write("1000000",X"FE")</t>
+  </si>
+  <si>
+    <t>Write("1110111",X"1E")</t>
+  </si>
+  <si>
+    <t>PTRH</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 1</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 2</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 3</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 4</t>
+  </si>
+  <si>
+    <t>0008</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 5</t>
+  </si>
+  <si>
+    <t>000A</t>
+  </si>
+  <si>
+    <t>MS5607 Coefficient 6</t>
+  </si>
+  <si>
+    <t>000C</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>000E</t>
+  </si>
+  <si>
+    <t>SHT21 Temperature</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>SHT21 Relative Humidity</t>
+  </si>
+  <si>
+    <t>0012</t>
+  </si>
+  <si>
+    <t>MS5607 P D1(15:0)</t>
+  </si>
+  <si>
+    <t>0014</t>
+  </si>
+  <si>
+    <t>MS5607 P D1(23:16)</t>
+  </si>
+  <si>
+    <t>0016</t>
+  </si>
+  <si>
+    <t>MS5607 T D2(15:0)</t>
+  </si>
+  <si>
+    <t>0018</t>
+  </si>
+  <si>
+    <t>MS5607 T D2(23:16)</t>
+  </si>
+  <si>
+    <t>Base Address</t>
+  </si>
+  <si>
+    <t>Carbon:</t>
+  </si>
+  <si>
+    <t>0200</t>
+  </si>
+  <si>
+    <t>DACS PTRH</t>
+  </si>
+  <si>
+    <t>0220</t>
+  </si>
+  <si>
+    <t>0240</t>
+  </si>
+  <si>
+    <t>0260</t>
+  </si>
+  <si>
+    <t>0280</t>
+  </si>
+  <si>
+    <t>02A0</t>
+  </si>
+  <si>
+    <t>02C0</t>
+  </si>
+  <si>
+    <t>02E0</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <t>0320</t>
+  </si>
+  <si>
+    <t>Disable everything on the old switch</t>
+  </si>
+  <si>
+    <t>Error here is is a problem if ISwitchBit(CurESID) = ISwitchBit(ESID(PTRHn))</t>
+  </si>
+  <si>
+    <t>Error here is always a problem</t>
+  </si>
+  <si>
+    <t>Save to Reg 7</t>
+  </si>
+  <si>
+    <t>Save to Regs 9 &amp; 10</t>
+  </si>
+  <si>
+    <t>Save to Reg 8</t>
+  </si>
+  <si>
+    <t>Save to Reg 11 &amp; 12</t>
+  </si>
+  <si>
+    <t>Update Status Word Reg 6</t>
+  </si>
+  <si>
+    <t>Read2(40,F3)</t>
+  </si>
+  <si>
+    <t>Read2(40)</t>
   </si>
 </sst>
 </file>
@@ -403,7 +568,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -572,6 +743,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,6 +765,116 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086475" y="13649325"/>
+          <a:ext cx="4391025" cy="1895475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Possible</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> failure modes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  Mux is non-existant or dead.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>      May as well hope for the best on deselection</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  Transient communication failure.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>      Would not want to read from any other devices on the same bus. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>      This is not currently an issue, since the switch is the only device on</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>      the bus.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -868,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView topLeftCell="G34" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -919,10 +1215,10 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" s="1"/>
@@ -2386,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:H76"/>
+  <dimension ref="A3:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2412,349 +2708,424 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="C6" t="s">
+    <row r="7" spans="1:8">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>47</v>
+      <c r="H7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="C17" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="C18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="D19" t="s">
+    <row r="20" spans="1:6">
+      <c r="D20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="E20" t="s">
+    <row r="21" spans="1:6">
+      <c r="E21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="F21" t="s">
+    <row r="22" spans="1:6">
+      <c r="F22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="E22" t="s">
+    <row r="23" spans="1:6">
+      <c r="E23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="F23" t="s">
+    <row r="24" spans="1:6">
+      <c r="F24" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="B31" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="B32" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="C37" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="C38" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="C39" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="2:3">
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="C41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="C42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="43" spans="2:3">
-      <c r="B43" t="s">
-        <v>73</v>
+      <c r="C43" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="2:3">
-      <c r="B44" t="s">
-        <v>68</v>
+      <c r="C44" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="2:3">
-      <c r="C46" t="s">
-        <v>80</v>
+      <c r="B46" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="2:3">
-      <c r="C47" t="s">
-        <v>74</v>
+      <c r="B47" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="2:3">
-      <c r="C48" t="s">
-        <v>75</v>
+      <c r="B48" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="B49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="B50" t="s">
-        <v>66</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="C51" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>81</v>
+      <c r="C52" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="B53" t="s">
-        <v>48</v>
+      <c r="C53" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="C54" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="D55" t="s">
-        <v>50</v>
+      <c r="C55" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="D56" t="s">
-        <v>82</v>
+      <c r="C56" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="E57" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="D58" t="s">
-        <v>64</v>
+      <c r="C57" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="E59" t="s">
-        <v>54</v>
+      <c r="A59" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="B60" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="C61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="D62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="D63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="E64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="D65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="E66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="C68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="B62" t="s">
+    <row r="69" spans="1:13">
+      <c r="B69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="C63" t="s">
+    <row r="70" spans="1:13">
+      <c r="C70" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
-      <c r="B64" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
+    <row r="71" spans="1:13">
+      <c r="B71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="B74" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="C75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="D76" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="D77" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="E78" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+      <c r="J78" s="23"/>
+      <c r="K78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="M78" s="23"/>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="C79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="B67" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="C68" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="D69" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="C70" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="C71" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="C72" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="B73" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="C74" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="C75" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="C76" t="s">
-        <v>83</v>
-      </c>
+    <row r="80" spans="1:13">
+      <c r="C80" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="C81" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="C83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="C85" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="D86" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E78:M78"/>
+    <mergeCell ref="D86:I86"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
@@ -2773,7 +3144,7 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -2877,10 +3248,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -2947,7 +3318,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2955,13 +3326,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="C22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2969,10 +3340,10 @@
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2980,35 +3351,329 @@
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="C25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>103</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <f>A33+1</f>
+        <v>1</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <f t="shared" ref="A35:A45" si="0">A34+1</f>
+        <v>2</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="20"/>
+      <c r="B46" s="16"/>
+      <c r="D46" s="16"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="16"/>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="16"/>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="16"/>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="16"/>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" s="16"/>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="16"/>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="16"/>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B33:B45 B48:B57" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>